<commit_message>
ajustando la logica para realizar manejo de errores
</commit_message>
<xml_diff>
--- a/resultado.xlsx
+++ b/resultado.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,29 +555,29 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>84346</v>
+        <v>84410</v>
       </c>
       <c r="B3" t="n">
-        <v>53068031</v>
+        <v>53068043</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Idiomas: B2:Inglés intermedio, N13 (J-Ad13+)</t>
+          <t>Idiomas: B2:Inglés intermedio, N14 (J-Ad13+)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Oscar Alexander Munera Agudelo</t>
+          <t>Daniel Guarin Acevedo</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OscarMunera@comfama.com.co</t>
+          <t>DanielGuarin@comfama.com.co</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Clase 20 - 53068031</t>
+          <t>Clase 20 - 53068043</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
@@ -589,49 +589,45 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>8236</v>
+        <v>8300</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Clase 20 - 53068031</t>
+          <t>Clase 20 - 53068043</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://comfama.webex.com/comfama/ldr.php?RCID=0e52207f7e212f8fa9bc838eef56d23c</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>https://sagrabacionescursos.blob.core.windows.net/videos/Clase 20 - 53068031-20211127 1259-1.mp4</t>
-        </is>
-      </c>
+          <t>https://comfama.webex.com/comfama/ldr.php?RCID=24172b94001615a9f9924cc1be32e5eddd</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>84449</v>
+        <v>825</v>
       </c>
       <c r="B4" t="n">
-        <v>53068051</v>
+        <v>53068027</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Idiomas: A2:Inglés básico, N4 (J-Ad13+)</t>
+          <t>Idiomas: B2:Inglés intermedio, N12 (J-Ad13+)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JULIAN HURTADO</t>
+          <t>EDWIN FERNANDO CARDONA BOCANEGRA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>julianhurtado@comfama.com.co</t>
+          <t>EdwinCardona@comfama.com.co</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Clase 19 - 53068051</t>
+          <t>Clase 19 - 53068027</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
@@ -639,133 +635,25 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>13:30:00</t>
+          <t>09:30:00</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>8339</v>
+        <v>8215</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Clase 19 - 53068051</t>
+          <t>Clase 19 - 53068027</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://comfama.webex.com/comfama/ldr.php?RCID=7b61fb0d40b4551f7d3422058e54611f</t>
+          <t>https://comfama.webex.com/comfama/ldr.php?RCID=ca7c616fa8a60ac9d71dbc710d76906c</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>https://sagrabacionescursos.blob.core.windows.net/videos/Clase 19 - 53068051-20211127 1840-1.mp4</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>84470</v>
-      </c>
-      <c r="B5" t="n">
-        <v>53068055</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Idiomas: B2:Inglés intermedio, N15 (J-Ad13+)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Yoeimis Paola Polo Gutiérrez</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>YoeimisPolo@comfama.com.co</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clase 20 - 53068055</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>44527</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>09:30:00</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>8360</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Clase 20 - 53068055</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>https://comfama.webex.com/comfama/ldr.php?RCID=89c0e2e34c9e0ecbbbb3051d1027ddfc</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>https://sagrabacionescursos.blob.core.windows.net/videos/Clase 20 - 53068055-20211127 1445-1.mp4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>84509</v>
-      </c>
-      <c r="B6" t="n">
-        <v>53068063</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Idiomas: B1:Inglés pre-intermedio, N9(10-12 años)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>tarkus laverde rojas</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>TarkusLaverde@comfama.com.co</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Clase 20 - 53068063</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>44527</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>09:30:00</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>8399</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Clase 20 - 53068063</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>https://comfama.webex.com/comfama/ldr.php?RCID=d29aefdffbab84b701f24f96c1da7528</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>https://sagrabacionescursos.blob.core.windows.net/videos/Clase 20 - 53068063-20211127 1500-1.mp4</t>
+          <t>https://sagrabacionescursos.blob.core.windows.net/videos/Clase 19 - 53068027-20211127 1455-1.mp4</t>
         </is>
       </c>
     </row>

</xml_diff>